<commit_message>
Add Plotly Dash app, update notebook and map data
</commit_message>
<xml_diff>
--- a/casemapdata.xlsx
+++ b/casemapdata.xlsx
@@ -1524,7 +1524,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>57534</v>
+        <v>57612</v>
       </c>
       <c r="C2" t="s">
         <v>190</v>
@@ -1535,7 +1535,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>129128</v>
+        <v>129307</v>
       </c>
       <c r="C3" t="s">
         <v>191</v>
@@ -1546,7 +1546,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>119142</v>
+        <v>119323</v>
       </c>
       <c r="C4" t="s">
         <v>192</v>
@@ -1557,7 +1557,7 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>12641</v>
+        <v>12712</v>
       </c>
       <c r="C5" t="s">
         <v>193</v>
@@ -1568,7 +1568,7 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>23951</v>
+        <v>24122</v>
       </c>
       <c r="C6" t="s">
         <v>194</v>
@@ -1579,7 +1579,7 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>1209</v>
+        <v>1213</v>
       </c>
       <c r="C7" t="s">
         <v>195</v>
@@ -1590,7 +1590,7 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>2629156</v>
+        <v>2658628</v>
       </c>
       <c r="C8" t="s">
         <v>196</v>
@@ -1601,7 +1601,7 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>206142</v>
+        <v>207103</v>
       </c>
       <c r="C9" t="s">
         <v>197</v>
@@ -1612,7 +1612,7 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>29484</v>
+        <v>29499</v>
       </c>
       <c r="C10" t="s">
         <v>198</v>
@@ -1623,7 +1623,7 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>586883</v>
+        <v>589299</v>
       </c>
       <c r="C11" t="s">
         <v>199</v>
@@ -1634,7 +1634,7 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>294211</v>
+        <v>296374</v>
       </c>
       <c r="C12" t="s">
         <v>200</v>
@@ -1645,7 +1645,7 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>9505</v>
+        <v>9634</v>
       </c>
       <c r="C13" t="s">
         <v>201</v>
@@ -1656,7 +1656,7 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>160934</v>
+        <v>162089</v>
       </c>
       <c r="C14" t="s">
         <v>202</v>
@@ -1667,7 +1667,7 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>707362</v>
+        <v>711779</v>
       </c>
       <c r="C15" t="s">
         <v>203</v>
@@ -1678,7 +1678,7 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <v>3753</v>
+        <v>3765</v>
       </c>
       <c r="C16" t="s">
         <v>204</v>
@@ -1689,7 +1689,7 @@
         <v>18</v>
       </c>
       <c r="B17">
-        <v>340023</v>
+        <v>341539</v>
       </c>
       <c r="C17" t="s">
         <v>205</v>
@@ -1700,7 +1700,7 @@
         <v>19</v>
       </c>
       <c r="B18">
-        <v>939309</v>
+        <v>943213</v>
       </c>
       <c r="C18" t="s">
         <v>206</v>
@@ -1711,7 +1711,7 @@
         <v>20</v>
       </c>
       <c r="B19">
-        <v>12529</v>
+        <v>12538</v>
       </c>
       <c r="C19" t="s">
         <v>207</v>
@@ -1733,7 +1733,7 @@
         <v>22</v>
       </c>
       <c r="B21">
-        <v>934</v>
+        <v>941</v>
       </c>
       <c r="C21" t="s">
         <v>209</v>
@@ -1744,7 +1744,7 @@
         <v>23</v>
       </c>
       <c r="B22">
-        <v>286114</v>
+        <v>287360</v>
       </c>
       <c r="C22" t="s">
         <v>210</v>
@@ -1755,7 +1755,7 @@
         <v>24</v>
       </c>
       <c r="B23">
-        <v>187715</v>
+        <v>188994</v>
       </c>
       <c r="C23" t="s">
         <v>211</v>
@@ -1777,7 +1777,7 @@
         <v>26</v>
       </c>
       <c r="B25">
-        <v>13746681</v>
+        <v>13832455</v>
       </c>
       <c r="C25" t="s">
         <v>213</v>
@@ -1799,7 +1799,7 @@
         <v>28</v>
       </c>
       <c r="B27">
-        <v>382761</v>
+        <v>384887</v>
       </c>
       <c r="C27" t="s">
         <v>215</v>
@@ -1810,7 +1810,7 @@
         <v>29</v>
       </c>
       <c r="B28">
-        <v>13064</v>
+        <v>13083</v>
       </c>
       <c r="C28" t="s">
         <v>216</v>
@@ -1821,7 +1821,7 @@
         <v>30</v>
       </c>
       <c r="B29">
-        <v>142610</v>
+        <v>142617</v>
       </c>
       <c r="C29" t="s">
         <v>217</v>
@@ -1832,7 +1832,7 @@
         <v>31</v>
       </c>
       <c r="B30">
-        <v>3424</v>
+        <v>3477</v>
       </c>
       <c r="C30" t="s">
         <v>218</v>
@@ -1843,7 +1843,7 @@
         <v>32</v>
       </c>
       <c r="B31">
-        <v>19780</v>
+        <v>19975</v>
       </c>
       <c r="C31" t="s">
         <v>219</v>
@@ -1854,7 +1854,7 @@
         <v>33</v>
       </c>
       <c r="B32">
-        <v>5218</v>
+        <v>5480</v>
       </c>
       <c r="C32" t="s">
         <v>220</v>
@@ -1876,7 +1876,7 @@
         <v>35</v>
       </c>
       <c r="B34">
-        <v>1104508</v>
+        <v>1113837</v>
       </c>
       <c r="C34" t="s">
         <v>222</v>
@@ -1887,7 +1887,7 @@
         <v>36</v>
       </c>
       <c r="B35">
-        <v>5682</v>
+        <v>5728</v>
       </c>
       <c r="C35" t="s">
         <v>223</v>
@@ -1898,7 +1898,7 @@
         <v>37</v>
       </c>
       <c r="B36">
-        <v>4673</v>
+        <v>4686</v>
       </c>
       <c r="C36" t="s">
         <v>224</v>
@@ -1909,7 +1909,7 @@
         <v>38</v>
       </c>
       <c r="B37">
-        <v>1101698</v>
+        <v>1109311</v>
       </c>
       <c r="C37" t="s">
         <v>225</v>
@@ -1920,7 +1920,7 @@
         <v>39</v>
       </c>
       <c r="B38">
-        <v>102135</v>
+        <v>102167</v>
       </c>
       <c r="C38" t="s">
         <v>226</v>
@@ -1931,7 +1931,7 @@
         <v>40</v>
       </c>
       <c r="B39">
-        <v>2602719</v>
+        <v>2619422</v>
       </c>
       <c r="C39" t="s">
         <v>227</v>
@@ -1942,7 +1942,7 @@
         <v>41</v>
       </c>
       <c r="B40">
-        <v>3809</v>
+        <v>3815</v>
       </c>
       <c r="C40" t="s">
         <v>228</v>
@@ -1964,7 +1964,7 @@
         <v>43</v>
       </c>
       <c r="B42">
-        <v>28769</v>
+        <v>28859</v>
       </c>
       <c r="C42" t="s">
         <v>230</v>
@@ -1975,7 +1975,7 @@
         <v>44</v>
       </c>
       <c r="B43">
-        <v>227533</v>
+        <v>228577</v>
       </c>
       <c r="C43" t="s">
         <v>231</v>
@@ -1986,7 +1986,7 @@
         <v>45</v>
       </c>
       <c r="B44">
-        <v>45444</v>
+        <v>45474</v>
       </c>
       <c r="C44" t="s">
         <v>232</v>
@@ -1997,7 +1997,7 @@
         <v>46</v>
       </c>
       <c r="B45">
-        <v>300900</v>
+        <v>303598</v>
       </c>
       <c r="C45" t="s">
         <v>233</v>
@@ -2008,7 +2008,7 @@
         <v>47</v>
       </c>
       <c r="B46">
-        <v>90408</v>
+        <v>91448</v>
       </c>
       <c r="C46" t="s">
         <v>234</v>
@@ -2019,7 +2019,7 @@
         <v>48</v>
       </c>
       <c r="B47">
-        <v>53944</v>
+        <v>54621</v>
       </c>
       <c r="C47" t="s">
         <v>235</v>
@@ -2030,7 +2030,7 @@
         <v>49</v>
       </c>
       <c r="B48">
-        <v>1593847</v>
+        <v>1597103</v>
       </c>
       <c r="C48" t="s">
         <v>236</v>
@@ -2041,7 +2041,7 @@
         <v>50</v>
       </c>
       <c r="B49">
-        <v>241023</v>
+        <v>241700</v>
       </c>
       <c r="C49" t="s">
         <v>237</v>
@@ -2052,7 +2052,7 @@
         <v>51</v>
       </c>
       <c r="B50">
-        <v>10275</v>
+        <v>10385</v>
       </c>
       <c r="C50" t="s">
         <v>238</v>
@@ -2074,7 +2074,7 @@
         <v>53</v>
       </c>
       <c r="B52">
-        <v>259639</v>
+        <v>260133</v>
       </c>
       <c r="C52" t="s">
         <v>240</v>
@@ -2085,7 +2085,7 @@
         <v>54</v>
       </c>
       <c r="B53">
-        <v>355431</v>
+        <v>355964</v>
       </c>
       <c r="C53" t="s">
         <v>241</v>
@@ -2096,7 +2096,7 @@
         <v>55</v>
       </c>
       <c r="B54">
-        <v>213798</v>
+        <v>214639</v>
       </c>
       <c r="C54" t="s">
         <v>242</v>
@@ -2107,7 +2107,7 @@
         <v>56</v>
       </c>
       <c r="B55">
-        <v>67099</v>
+        <v>67249</v>
       </c>
       <c r="C55" t="s">
         <v>243</v>
@@ -2129,7 +2129,7 @@
         <v>58</v>
       </c>
       <c r="B57">
-        <v>3486</v>
+        <v>3491</v>
       </c>
       <c r="C57" t="s">
         <v>245</v>
@@ -2140,7 +2140,7 @@
         <v>59</v>
       </c>
       <c r="B58">
-        <v>116200</v>
+        <v>116678</v>
       </c>
       <c r="C58" t="s">
         <v>246</v>
@@ -2151,7 +2151,7 @@
         <v>60</v>
       </c>
       <c r="B59">
-        <v>18412</v>
+        <v>18414</v>
       </c>
       <c r="C59" t="s">
         <v>247</v>
@@ -2162,7 +2162,7 @@
         <v>61</v>
       </c>
       <c r="B60">
-        <v>236554</v>
+        <v>238527</v>
       </c>
       <c r="C60" t="s">
         <v>248</v>
@@ -2184,7 +2184,7 @@
         <v>63</v>
       </c>
       <c r="B62">
-        <v>83253</v>
+        <v>83633</v>
       </c>
       <c r="C62" t="s">
         <v>250</v>
@@ -2195,7 +2195,7 @@
         <v>64</v>
       </c>
       <c r="B63">
-        <v>5248853</v>
+        <v>5285304</v>
       </c>
       <c r="C63" t="s">
         <v>251</v>
@@ -2217,7 +2217,7 @@
         <v>66</v>
       </c>
       <c r="B65">
-        <v>5694</v>
+        <v>5720</v>
       </c>
       <c r="C65" t="s">
         <v>253</v>
@@ -2228,7 +2228,7 @@
         <v>67</v>
       </c>
       <c r="B66">
-        <v>292244</v>
+        <v>293321</v>
       </c>
       <c r="C66" t="s">
         <v>254</v>
@@ -2239,7 +2239,7 @@
         <v>68</v>
       </c>
       <c r="B67">
-        <v>3110252</v>
+        <v>3134108</v>
       </c>
       <c r="C67" t="s">
         <v>255</v>
@@ -2261,7 +2261,7 @@
         <v>70</v>
       </c>
       <c r="B69">
-        <v>308006</v>
+        <v>311033</v>
       </c>
       <c r="C69" t="s">
         <v>257</v>
@@ -2283,7 +2283,7 @@
         <v>72</v>
       </c>
       <c r="B71">
-        <v>208694</v>
+        <v>210667</v>
       </c>
       <c r="C71" t="s">
         <v>259</v>
@@ -2294,7 +2294,7 @@
         <v>73</v>
       </c>
       <c r="B72">
-        <v>21299</v>
+        <v>21392</v>
       </c>
       <c r="C72" t="s">
         <v>260</v>
@@ -2305,7 +2305,7 @@
         <v>74</v>
       </c>
       <c r="B73">
-        <v>3706</v>
+        <v>3710</v>
       </c>
       <c r="C73" t="s">
         <v>261</v>
@@ -2316,7 +2316,7 @@
         <v>75</v>
       </c>
       <c r="B74">
-        <v>11527</v>
+        <v>11642</v>
       </c>
       <c r="C74" t="s">
         <v>262</v>
@@ -2327,7 +2327,7 @@
         <v>76</v>
       </c>
       <c r="B75">
-        <v>12857</v>
+        <v>12876</v>
       </c>
       <c r="C75" t="s">
         <v>263</v>
@@ -2338,7 +2338,7 @@
         <v>77</v>
       </c>
       <c r="B76">
-        <v>198975</v>
+        <v>199682</v>
       </c>
       <c r="C76" t="s">
         <v>264</v>
@@ -2349,7 +2349,7 @@
         <v>78</v>
       </c>
       <c r="B77">
-        <v>736982</v>
+        <v>742198</v>
       </c>
       <c r="C77" t="s">
         <v>265</v>
@@ -2360,7 +2360,7 @@
         <v>79</v>
       </c>
       <c r="B78">
-        <v>6279</v>
+        <v>6286</v>
       </c>
       <c r="C78" t="s">
         <v>266</v>
@@ -2371,7 +2371,7 @@
         <v>80</v>
       </c>
       <c r="B79">
-        <v>14291917</v>
+        <v>14526609</v>
       </c>
       <c r="C79" t="s">
         <v>267</v>
@@ -2382,7 +2382,7 @@
         <v>81</v>
       </c>
       <c r="B80">
-        <v>1589359</v>
+        <v>1594722</v>
       </c>
       <c r="C80" t="s">
         <v>268</v>
@@ -2393,7 +2393,7 @@
         <v>82</v>
       </c>
       <c r="B81">
-        <v>2168872</v>
+        <v>2194133</v>
       </c>
       <c r="C81" t="s">
         <v>269</v>
@@ -2404,7 +2404,7 @@
         <v>83</v>
       </c>
       <c r="B82">
-        <v>956860</v>
+        <v>964435</v>
       </c>
       <c r="C82" t="s">
         <v>270</v>
@@ -2415,7 +2415,7 @@
         <v>84</v>
       </c>
       <c r="B83">
-        <v>242402</v>
+        <v>242819</v>
       </c>
       <c r="C83" t="s">
         <v>271</v>
@@ -2426,7 +2426,7 @@
         <v>85</v>
       </c>
       <c r="B84">
-        <v>836902</v>
+        <v>836936</v>
       </c>
       <c r="C84" t="s">
         <v>272</v>
@@ -2437,7 +2437,7 @@
         <v>86</v>
       </c>
       <c r="B85">
-        <v>3826156</v>
+        <v>3842079</v>
       </c>
       <c r="C85" t="s">
         <v>273</v>
@@ -2448,7 +2448,7 @@
         <v>87</v>
       </c>
       <c r="B86">
-        <v>43240</v>
+        <v>43473</v>
       </c>
       <c r="C86" t="s">
         <v>274</v>
@@ -2459,7 +2459,7 @@
         <v>88</v>
       </c>
       <c r="B87">
-        <v>521796</v>
+        <v>526307</v>
       </c>
       <c r="C87" t="s">
         <v>275</v>
@@ -2470,7 +2470,7 @@
         <v>89</v>
       </c>
       <c r="B88">
-        <v>679138</v>
+        <v>681870</v>
       </c>
       <c r="C88" t="s">
         <v>276</v>
@@ -2481,7 +2481,7 @@
         <v>90</v>
       </c>
       <c r="B89">
-        <v>333046</v>
+        <v>335868</v>
       </c>
       <c r="C89" t="s">
         <v>277</v>
@@ -2492,7 +2492,7 @@
         <v>91</v>
       </c>
       <c r="B90">
-        <v>149219</v>
+        <v>150260</v>
       </c>
       <c r="C90" t="s">
         <v>278</v>
@@ -2503,7 +2503,7 @@
         <v>92</v>
       </c>
       <c r="B91">
-        <v>112789</v>
+        <v>113444</v>
       </c>
       <c r="C91" t="s">
         <v>279</v>
@@ -2514,7 +2514,7 @@
         <v>93</v>
       </c>
       <c r="B92">
-        <v>99210</v>
+        <v>100329</v>
       </c>
       <c r="C92" t="s">
         <v>280</v>
@@ -2525,7 +2525,7 @@
         <v>94</v>
       </c>
       <c r="B93">
-        <v>253066</v>
+        <v>254472</v>
       </c>
       <c r="C93" t="s">
         <v>281</v>
@@ -2536,7 +2536,7 @@
         <v>95</v>
       </c>
       <c r="B94">
-        <v>91144</v>
+        <v>91374</v>
       </c>
       <c r="C94" t="s">
         <v>282</v>
@@ -2547,7 +2547,7 @@
         <v>96</v>
       </c>
       <c r="B95">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C95" t="s">
         <v>283</v>
@@ -2558,7 +2558,7 @@
         <v>97</v>
       </c>
       <c r="B96">
-        <v>109731</v>
+        <v>110343</v>
       </c>
       <c r="C96" t="s">
         <v>284</v>
@@ -2569,7 +2569,7 @@
         <v>98</v>
       </c>
       <c r="B97">
-        <v>504800</v>
+        <v>506808</v>
       </c>
       <c r="C97" t="s">
         <v>285</v>
@@ -2602,7 +2602,7 @@
         <v>101</v>
       </c>
       <c r="B100">
-        <v>170558</v>
+        <v>171131</v>
       </c>
       <c r="C100" t="s">
         <v>288</v>
@@ -2613,7 +2613,7 @@
         <v>102</v>
       </c>
       <c r="B101">
-        <v>2780</v>
+        <v>2790</v>
       </c>
       <c r="C101" t="s">
         <v>289</v>
@@ -2624,7 +2624,7 @@
         <v>103</v>
       </c>
       <c r="B102">
-        <v>230462</v>
+        <v>231601</v>
       </c>
       <c r="C102" t="s">
         <v>290</v>
@@ -2635,7 +2635,7 @@
         <v>104</v>
       </c>
       <c r="B103">
-        <v>64549</v>
+        <v>64746</v>
       </c>
       <c r="C103" t="s">
         <v>291</v>
@@ -2646,7 +2646,7 @@
         <v>105</v>
       </c>
       <c r="B104">
-        <v>30207</v>
+        <v>31039</v>
       </c>
       <c r="C104" t="s">
         <v>292</v>
@@ -2657,7 +2657,7 @@
         <v>106</v>
       </c>
       <c r="B105">
-        <v>33902</v>
+        <v>33919</v>
       </c>
       <c r="C105" t="s">
         <v>293</v>
@@ -2668,7 +2668,7 @@
         <v>107</v>
       </c>
       <c r="B106">
-        <v>367977</v>
+        <v>370528</v>
       </c>
       <c r="C106" t="s">
         <v>294</v>
@@ -2679,7 +2679,7 @@
         <v>108</v>
       </c>
       <c r="B107">
-        <v>25939</v>
+        <v>26021</v>
       </c>
       <c r="C107" t="s">
         <v>295</v>
@@ -2690,7 +2690,7 @@
         <v>109</v>
       </c>
       <c r="B108">
-        <v>12706</v>
+        <v>12835</v>
       </c>
       <c r="C108" t="s">
         <v>296</v>
@@ -2701,7 +2701,7 @@
         <v>110</v>
       </c>
       <c r="B109">
-        <v>29833</v>
+        <v>29860</v>
       </c>
       <c r="C109" t="s">
         <v>297</v>
@@ -2723,7 +2723,7 @@
         <v>112</v>
       </c>
       <c r="B111">
-        <v>18072</v>
+        <v>18103</v>
       </c>
       <c r="C111" t="s">
         <v>299</v>
@@ -2745,7 +2745,7 @@
         <v>114</v>
       </c>
       <c r="B113">
-        <v>2295435</v>
+        <v>2299939</v>
       </c>
       <c r="C113" t="s">
         <v>301</v>
@@ -2756,7 +2756,7 @@
         <v>115</v>
       </c>
       <c r="B114">
-        <v>244177</v>
+        <v>244866</v>
       </c>
       <c r="C114" t="s">
         <v>302</v>
@@ -2767,7 +2767,7 @@
         <v>116</v>
       </c>
       <c r="B115">
-        <v>2387</v>
+        <v>2391</v>
       </c>
       <c r="C115" t="s">
         <v>303</v>
@@ -2778,7 +2778,7 @@
         <v>117</v>
       </c>
       <c r="B116">
-        <v>18565</v>
+        <v>19672</v>
       </c>
       <c r="C116" t="s">
         <v>304</v>
@@ -2789,7 +2789,7 @@
         <v>118</v>
       </c>
       <c r="B117">
-        <v>95042</v>
+        <v>95205</v>
       </c>
       <c r="C117" t="s">
         <v>305</v>
@@ -2800,7 +2800,7 @@
         <v>119</v>
       </c>
       <c r="B118">
-        <v>504260</v>
+        <v>504847</v>
       </c>
       <c r="C118" t="s">
         <v>306</v>
@@ -2811,7 +2811,7 @@
         <v>120</v>
       </c>
       <c r="B119">
-        <v>69002</v>
+        <v>69067</v>
       </c>
       <c r="C119" t="s">
         <v>307</v>
@@ -2822,7 +2822,7 @@
         <v>121</v>
       </c>
       <c r="B120">
-        <v>46185</v>
+        <v>46330</v>
       </c>
       <c r="C120" t="s">
         <v>308</v>
@@ -2833,7 +2833,7 @@
         <v>122</v>
       </c>
       <c r="B121">
-        <v>282054</v>
+        <v>282890</v>
       </c>
       <c r="C121" t="s">
         <v>309</v>
@@ -2844,7 +2844,7 @@
         <v>123</v>
       </c>
       <c r="B122">
-        <v>1402433</v>
+        <v>1411474</v>
       </c>
       <c r="C122" t="s">
         <v>310</v>
@@ -2877,7 +2877,7 @@
         <v>126</v>
       </c>
       <c r="B125">
-        <v>5113</v>
+        <v>5116</v>
       </c>
       <c r="C125" t="s">
         <v>313</v>
@@ -2888,7 +2888,7 @@
         <v>127</v>
       </c>
       <c r="B126">
-        <v>164080</v>
+        <v>164147</v>
       </c>
       <c r="C126" t="s">
         <v>314</v>
@@ -2899,7 +2899,7 @@
         <v>128</v>
       </c>
       <c r="B127">
-        <v>106224</v>
+        <v>106727</v>
       </c>
       <c r="C127" t="s">
         <v>315</v>
@@ -2921,7 +2921,7 @@
         <v>130</v>
       </c>
       <c r="B129">
-        <v>745182</v>
+        <v>750158</v>
       </c>
       <c r="C129" t="s">
         <v>317</v>
@@ -2932,7 +2932,7 @@
         <v>131</v>
       </c>
       <c r="B130">
-        <v>359830</v>
+        <v>360249</v>
       </c>
       <c r="C130" t="s">
         <v>318</v>
@@ -2943,7 +2943,7 @@
         <v>132</v>
       </c>
       <c r="B131">
-        <v>9188</v>
+        <v>9343</v>
       </c>
       <c r="C131" t="s">
         <v>319</v>
@@ -2965,7 +2965,7 @@
         <v>134</v>
       </c>
       <c r="B133">
-        <v>1667737</v>
+        <v>1681063</v>
       </c>
       <c r="C133" t="s">
         <v>321</v>
@@ -2976,7 +2976,7 @@
         <v>135</v>
       </c>
       <c r="B134">
-        <v>904285</v>
+        <v>914971</v>
       </c>
       <c r="C134" t="s">
         <v>322</v>
@@ -2987,7 +2987,7 @@
         <v>136</v>
       </c>
       <c r="B135">
-        <v>2642242</v>
+        <v>2660088</v>
       </c>
       <c r="C135" t="s">
         <v>323</v>
@@ -2998,7 +2998,7 @@
         <v>137</v>
       </c>
       <c r="B136">
-        <v>829358</v>
+        <v>829911</v>
       </c>
       <c r="C136" t="s">
         <v>324</v>
@@ -3009,7 +3009,7 @@
         <v>138</v>
       </c>
       <c r="B137">
-        <v>193952</v>
+        <v>194930</v>
       </c>
       <c r="C137" t="s">
         <v>325</v>
@@ -3020,7 +3020,7 @@
         <v>139</v>
       </c>
       <c r="B138">
-        <v>1020301</v>
+        <v>1023565</v>
       </c>
       <c r="C138" t="s">
         <v>326</v>
@@ -3031,7 +3031,7 @@
         <v>140</v>
       </c>
       <c r="B139">
-        <v>4622464</v>
+        <v>4631336</v>
       </c>
       <c r="C139" t="s">
         <v>327</v>
@@ -3042,7 +3042,7 @@
         <v>141</v>
       </c>
       <c r="B140">
-        <v>23744</v>
+        <v>23812</v>
       </c>
       <c r="C140" t="s">
         <v>328</v>
@@ -3064,7 +3064,7 @@
         <v>143</v>
       </c>
       <c r="B142">
-        <v>4355</v>
+        <v>4398</v>
       </c>
       <c r="C142" t="s">
         <v>330</v>
@@ -3075,7 +3075,7 @@
         <v>144</v>
       </c>
       <c r="B143">
-        <v>1818</v>
+        <v>1819</v>
       </c>
       <c r="C143" t="s">
         <v>331</v>
@@ -3097,7 +3097,7 @@
         <v>146</v>
       </c>
       <c r="B145">
-        <v>5010</v>
+        <v>5016</v>
       </c>
       <c r="C145" t="s">
         <v>333</v>
@@ -3108,7 +3108,7 @@
         <v>147</v>
       </c>
       <c r="B146">
-        <v>2271</v>
+        <v>2272</v>
       </c>
       <c r="C146" t="s">
         <v>334</v>
@@ -3119,7 +3119,7 @@
         <v>148</v>
       </c>
       <c r="B147">
-        <v>402142</v>
+        <v>403106</v>
       </c>
       <c r="C147" t="s">
         <v>335</v>
@@ -3130,7 +3130,7 @@
         <v>149</v>
       </c>
       <c r="B148">
-        <v>39606</v>
+        <v>39664</v>
       </c>
       <c r="C148" t="s">
         <v>336</v>
@@ -3141,7 +3141,7 @@
         <v>150</v>
       </c>
       <c r="B149">
-        <v>654870</v>
+        <v>657716</v>
       </c>
       <c r="C149" t="s">
         <v>337</v>
@@ -3152,7 +3152,7 @@
         <v>151</v>
       </c>
       <c r="B150">
-        <v>4765</v>
+        <v>4834</v>
       </c>
       <c r="C150" t="s">
         <v>338</v>
@@ -3174,7 +3174,7 @@
         <v>153</v>
       </c>
       <c r="B152">
-        <v>60735</v>
+        <v>60769</v>
       </c>
       <c r="C152" t="s">
         <v>340</v>
@@ -3185,7 +3185,7 @@
         <v>154</v>
       </c>
       <c r="B153">
-        <v>373950</v>
+        <v>374586</v>
       </c>
       <c r="C153" t="s">
         <v>341</v>
@@ -3196,7 +3196,7 @@
         <v>155</v>
       </c>
       <c r="B154">
-        <v>229967</v>
+        <v>230826</v>
       </c>
       <c r="C154" t="s">
         <v>342</v>
@@ -3207,7 +3207,7 @@
         <v>156</v>
       </c>
       <c r="B155">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C155" t="s">
         <v>343</v>
@@ -3229,7 +3229,7 @@
         <v>158</v>
       </c>
       <c r="B157">
-        <v>1562931</v>
+        <v>1564355</v>
       </c>
       <c r="C157" t="s">
         <v>345</v>
@@ -3240,7 +3240,7 @@
         <v>159</v>
       </c>
       <c r="B158">
-        <v>10416</v>
+        <v>10432</v>
       </c>
       <c r="C158" t="s">
         <v>346</v>
@@ -3251,7 +3251,7 @@
         <v>160</v>
       </c>
       <c r="B159">
-        <v>3396685</v>
+        <v>3407283</v>
       </c>
       <c r="C159" t="s">
         <v>347</v>
@@ -3262,7 +3262,7 @@
         <v>161</v>
       </c>
       <c r="B160">
-        <v>95949</v>
+        <v>96186</v>
       </c>
       <c r="C160" t="s">
         <v>348</v>
@@ -3273,7 +3273,7 @@
         <v>162</v>
       </c>
       <c r="B161">
-        <v>32932</v>
+        <v>33022</v>
       </c>
       <c r="C161" t="s">
         <v>349</v>
@@ -3284,7 +3284,7 @@
         <v>163</v>
       </c>
       <c r="B162">
-        <v>9458</v>
+        <v>9496</v>
       </c>
       <c r="C162" t="s">
         <v>350</v>
@@ -3295,7 +3295,7 @@
         <v>164</v>
       </c>
       <c r="B163">
-        <v>892480</v>
+        <v>900138</v>
       </c>
       <c r="C163" t="s">
         <v>351</v>
@@ -3306,7 +3306,7 @@
         <v>165</v>
       </c>
       <c r="B164">
-        <v>630194</v>
+        <v>632399</v>
       </c>
       <c r="C164" t="s">
         <v>352</v>
@@ -3317,7 +3317,7 @@
         <v>166</v>
       </c>
       <c r="B165">
-        <v>20713</v>
+        <v>20856</v>
       </c>
       <c r="C165" t="s">
         <v>353</v>
@@ -3328,7 +3328,7 @@
         <v>167</v>
       </c>
       <c r="B166">
-        <v>1068</v>
+        <v>1070</v>
       </c>
       <c r="C166" t="s">
         <v>354</v>
@@ -3361,7 +3361,7 @@
         <v>170</v>
       </c>
       <c r="B169">
-        <v>37453</v>
+        <v>39038</v>
       </c>
       <c r="C169" t="s">
         <v>357</v>
@@ -3372,7 +3372,7 @@
         <v>171</v>
       </c>
       <c r="B170">
-        <v>1138</v>
+        <v>1193</v>
       </c>
       <c r="C170" t="s">
         <v>358</v>
@@ -3383,7 +3383,7 @@
         <v>172</v>
       </c>
       <c r="B171">
-        <v>12214</v>
+        <v>12391</v>
       </c>
       <c r="C171" t="s">
         <v>359</v>
@@ -3405,7 +3405,7 @@
         <v>174</v>
       </c>
       <c r="B173">
-        <v>279376</v>
+        <v>281777</v>
       </c>
       <c r="C173" t="s">
         <v>361</v>
@@ -3416,7 +3416,7 @@
         <v>175</v>
       </c>
       <c r="B174">
-        <v>4086957</v>
+        <v>4150039</v>
       </c>
       <c r="C174" t="s">
         <v>362</v>
@@ -3427,7 +3427,7 @@
         <v>176</v>
       </c>
       <c r="B175">
-        <v>31495649</v>
+        <v>31575640</v>
       </c>
       <c r="C175" t="s">
         <v>363</v>
@@ -3438,7 +3438,7 @@
         <v>177</v>
       </c>
       <c r="B176">
-        <v>41263</v>
+        <v>41310</v>
       </c>
       <c r="C176" t="s">
         <v>364</v>
@@ -3449,7 +3449,7 @@
         <v>178</v>
       </c>
       <c r="B177">
-        <v>1956454</v>
+        <v>1974056</v>
       </c>
       <c r="C177" t="s">
         <v>365</v>
@@ -3460,7 +3460,7 @@
         <v>179</v>
       </c>
       <c r="B178">
-        <v>491423</v>
+        <v>493266</v>
       </c>
       <c r="C178" t="s">
         <v>366</v>
@@ -3471,7 +3471,7 @@
         <v>180</v>
       </c>
       <c r="B179">
-        <v>4396096</v>
+        <v>4398903</v>
       </c>
       <c r="C179" t="s">
         <v>367</v>
@@ -3482,7 +3482,7 @@
         <v>181</v>
       </c>
       <c r="B180">
-        <v>156499</v>
+        <v>159569</v>
       </c>
       <c r="C180" t="s">
         <v>368</v>
@@ -3493,7 +3493,7 @@
         <v>182</v>
       </c>
       <c r="B181">
-        <v>85730</v>
+        <v>86022</v>
       </c>
       <c r="C181" t="s">
         <v>369</v>
@@ -3515,7 +3515,7 @@
         <v>184</v>
       </c>
       <c r="B183">
-        <v>179365</v>
+        <v>180609</v>
       </c>
       <c r="C183" t="s">
         <v>371</v>
@@ -3526,7 +3526,7 @@
         <v>185</v>
       </c>
       <c r="B184">
-        <v>2758</v>
+        <v>2772</v>
       </c>
       <c r="C184" t="s">
         <v>372</v>
@@ -3537,7 +3537,7 @@
         <v>186</v>
       </c>
       <c r="B185">
-        <v>276407</v>
+        <v>278135</v>
       </c>
       <c r="C185" t="s">
         <v>373</v>
@@ -3548,7 +3548,7 @@
         <v>187</v>
       </c>
       <c r="B186">
-        <v>5657</v>
+        <v>5715</v>
       </c>
       <c r="C186" t="s">
         <v>374</v>
@@ -3559,7 +3559,7 @@
         <v>188</v>
       </c>
       <c r="B187">
-        <v>90532</v>
+        <v>90750</v>
       </c>
       <c r="C187" t="s">
         <v>375</v>
@@ -3570,7 +3570,7 @@
         <v>189</v>
       </c>
       <c r="B188">
-        <v>37422</v>
+        <v>37534</v>
       </c>
       <c r="C188" t="s">
         <v>376</v>

</xml_diff>

<commit_message>
Modified Data from pre-processor module
</commit_message>
<xml_diff>
--- a/casemapdata.xlsx
+++ b/casemapdata.xlsx
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>60122</v>
+        <v>60300</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>131238</v>
+        <v>131276</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -487,7 +487,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>122522</v>
+        <v>122717</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>13282</v>
+        <v>13295</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>26993</v>
+        <v>27133</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -547,7 +547,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>3005259</v>
+        <v>3021179</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>216863</v>
+        <v>217008</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -577,7 +577,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>29838</v>
+        <v>29850</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>622110</v>
+        <v>623201</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -607,7 +607,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>321380</v>
+        <v>321798</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>10519</v>
+        <v>10576</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>179297</v>
+        <v>180462</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>761943</v>
+        <v>763682</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -667,7 +667,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>3866</v>
+        <v>3881</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>361063</v>
+        <v>361897</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -697,7 +697,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>995562</v>
+        <v>996896</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>12668</v>
+        <v>12674</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -727,7 +727,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>7821</v>
+        <v>7884</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -757,7 +757,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>306527</v>
+        <v>308984</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -787,7 +787,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>46934</v>
+        <v>47851</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -802,7 +802,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>14754910</v>
+        <v>14779529</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>405194</v>
+        <v>405825</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -847,7 +847,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>13319</v>
+        <v>13324</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>142838</v>
+        <v>142842</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -877,7 +877,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>4038</v>
+        <v>4046</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -892,7 +892,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>24368</v>
+        <v>24548</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -907,7 +907,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>14520</v>
+        <v>15361</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -937,7 +937,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1240878</v>
+        <v>1251811</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -982,7 +982,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>1210920</v>
+        <v>1215815</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -997,7 +997,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>102530</v>
+        <v>102549</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1012,7 +1012,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>2893655</v>
+        <v>2905254</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1027,7 +1027,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>3839</v>
+        <v>3845</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1042,7 +1042,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>10678</v>
+        <v>11016</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1057,7 +1057,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>29965</v>
+        <v>30004</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1072,7 +1072,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>250991</v>
+        <v>256676</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1087,7 +1087,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>46114</v>
+        <v>46154</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1102,7 +1102,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>335173</v>
+        <v>335522</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1117,7 +1117,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>108693</v>
+        <v>109625</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>66372</v>
+        <v>66911</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1147,7 +1147,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>1634114</v>
+        <v>1634619</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>253607</v>
+        <v>254368</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1177,7 +1177,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>11157</v>
+        <v>11201</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1207,7 +1207,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>267455</v>
+        <v>267681</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>387299</v>
+        <v>388046</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>229635</v>
+        <v>230713</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1252,7 +1252,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>69198</v>
+        <v>69727</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1282,7 +1282,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>3671</v>
+        <v>3673</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1297,7 +1297,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>122685</v>
+        <v>122943</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -1312,7 +1312,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>18458</v>
+        <v>18460</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1327,7 +1327,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>258384</v>
+        <v>258813</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1342,7 +1342,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1357,7 +1357,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>87228</v>
+        <v>87345</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1372,7 +1372,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>5713393</v>
+        <v>5717160</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -1387,7 +1387,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>23075</v>
+        <v>23201</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -1417,7 +1417,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>312445</v>
+        <v>312954</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1432,7 +1432,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>3432676</v>
+        <v>3438186</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -1447,7 +1447,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>92601</v>
+        <v>92683</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -1462,7 +1462,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>346422</v>
+        <v>348568</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -1492,7 +1492,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>228684</v>
+        <v>228871</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -1507,7 +1507,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>22304</v>
+        <v>22333</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -1537,7 +1537,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>13518</v>
+        <v>13564</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -1567,7 +1567,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>213167</v>
+        <v>214475</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -1582,7 +1582,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>782892</v>
+        <v>784111</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -1597,7 +1597,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>6472</v>
+        <v>6483</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -1612,7 +1612,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>19925517</v>
+        <v>20282833</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -1627,7 +1627,7 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>1677274</v>
+        <v>1682004</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -1642,7 +1642,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>2534855</v>
+        <v>2555587</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -1657,7 +1657,7 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>1074930</v>
+        <v>1079998</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -1672,7 +1672,7 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>249838</v>
+        <v>250290</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -1687,7 +1687,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>838554</v>
+        <v>838621</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -1702,7 +1702,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>4044762</v>
+        <v>4050708</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -1717,7 +1717,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>45867</v>
+        <v>46039</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -1732,7 +1732,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>605150</v>
+        <v>609625</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -1747,7 +1747,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>712901</v>
+        <v>714173</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -1762,7 +1762,7 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>381078</v>
+        <v>383164</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -1777,7 +1777,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>160422</v>
+        <v>160559</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -1792,7 +1792,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>123728</v>
+        <v>124269</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -1822,7 +1822,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>276586</v>
+        <v>277832</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -1837,7 +1837,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>96060</v>
+        <v>96337</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -1852,7 +1852,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>933</v>
+        <v>966</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -1867,7 +1867,7 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>119750</v>
+        <v>119953</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -1882,7 +1882,7 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>528208</v>
+        <v>528457</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
@@ -1912,7 +1912,7 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>2099</v>
+        <v>2110</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
@@ -1927,7 +1927,7 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>177871</v>
+        <v>178335</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
@@ -1942,7 +1942,7 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>2940</v>
+        <v>2946</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
@@ -1957,7 +1957,7 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>249680</v>
+        <v>250337</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
@@ -1972,7 +1972,7 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>67205</v>
+        <v>67495</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
@@ -1987,7 +1987,7 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>37630</v>
+        <v>37751</v>
       </c>
       <c r="C104" t="inlineStr">
         <is>
@@ -2002,7 +2002,7 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>34096</v>
+        <v>34099</v>
       </c>
       <c r="C105" t="inlineStr">
         <is>
@@ -2017,7 +2017,7 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>415012</v>
+        <v>417512</v>
       </c>
       <c r="C106" t="inlineStr">
         <is>
@@ -2032,7 +2032,7 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>30745</v>
+        <v>31330</v>
       </c>
       <c r="C107" t="inlineStr">
         <is>
@@ -2047,7 +2047,7 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>13915</v>
+        <v>13937</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
@@ -2062,7 +2062,7 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>30319</v>
+        <v>30354</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
@@ -2092,7 +2092,7 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>18448</v>
+        <v>18476</v>
       </c>
       <c r="C111" t="inlineStr">
         <is>
@@ -2122,7 +2122,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>2348873</v>
+        <v>2349900</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
@@ -2137,7 +2137,7 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>251335</v>
+        <v>251378</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
@@ -2152,7 +2152,7 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>2457</v>
+        <v>2465</v>
       </c>
       <c r="C115" t="inlineStr">
         <is>
@@ -2167,7 +2167,7 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>39381</v>
+        <v>40396</v>
       </c>
       <c r="C116" t="inlineStr">
         <is>
@@ -2182,7 +2182,7 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>97619</v>
+        <v>97718</v>
       </c>
       <c r="C117" t="inlineStr">
         <is>
@@ -2197,7 +2197,7 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>511856</v>
+        <v>511912</v>
       </c>
       <c r="C118" t="inlineStr">
         <is>
@@ -2212,7 +2212,7 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>69984</v>
+        <v>70000</v>
       </c>
       <c r="C119" t="inlineStr">
         <is>
@@ -2242,7 +2242,7 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>336030</v>
+        <v>343418</v>
       </c>
       <c r="C121" t="inlineStr">
         <is>
@@ -2257,7 +2257,7 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>1534264</v>
+        <v>1543494</v>
       </c>
       <c r="C122" t="inlineStr">
         <is>
@@ -2272,7 +2272,7 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>2622</v>
+        <v>2623</v>
       </c>
       <c r="C123" t="inlineStr">
         <is>
@@ -2302,7 +2302,7 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>5251</v>
+        <v>5261</v>
       </c>
       <c r="C125" t="inlineStr">
         <is>
@@ -2317,7 +2317,7 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>165153</v>
+        <v>165199</v>
       </c>
       <c r="C126" t="inlineStr">
         <is>
@@ -2332,7 +2332,7 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>113469</v>
+        <v>113952</v>
       </c>
       <c r="C127" t="inlineStr">
         <is>
@@ -2347,7 +2347,7 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>195807</v>
+        <v>196900</v>
       </c>
       <c r="C128" t="inlineStr">
         <is>
@@ -2362,7 +2362,7 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>834146</v>
+        <v>837523</v>
       </c>
       <c r="C129" t="inlineStr">
         <is>
@@ -2377,7 +2377,7 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>365104</v>
+        <v>365299</v>
       </c>
       <c r="C130" t="inlineStr">
         <is>
@@ -2392,7 +2392,7 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>11206</v>
+        <v>11262</v>
       </c>
       <c r="C131" t="inlineStr">
         <is>
@@ -2407,7 +2407,7 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>282543</v>
+        <v>284453</v>
       </c>
       <c r="C132" t="inlineStr">
         <is>
@@ -2422,7 +2422,7 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>1810998</v>
+        <v>1814127</v>
       </c>
       <c r="C133" t="inlineStr">
         <is>
@@ -2437,7 +2437,7 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>1054983</v>
+        <v>1062225</v>
       </c>
       <c r="C134" t="inlineStr">
         <is>
@@ -2452,7 +2452,7 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>2803233</v>
+        <v>2805756</v>
       </c>
       <c r="C135" t="inlineStr">
         <is>
@@ -2467,7 +2467,7 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>837277</v>
+        <v>837457</v>
       </c>
       <c r="C136" t="inlineStr">
         <is>
@@ -2482,7 +2482,7 @@
         </is>
       </c>
       <c r="B137" t="n">
-        <v>206948</v>
+        <v>207592</v>
       </c>
       <c r="C137" t="inlineStr">
         <is>
@@ -2497,7 +2497,7 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>1057655</v>
+        <v>1058337</v>
       </c>
       <c r="C138" t="inlineStr">
         <is>
@@ -2512,7 +2512,7 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>4768476</v>
+        <v>4776844</v>
       </c>
       <c r="C139" t="inlineStr">
         <is>
@@ -2527,7 +2527,7 @@
         </is>
       </c>
       <c r="B140" t="n">
-        <v>25253</v>
+        <v>25311</v>
       </c>
       <c r="C140" t="inlineStr">
         <is>
@@ -2602,7 +2602,7 @@
         </is>
       </c>
       <c r="B145" t="n">
-        <v>5066</v>
+        <v>5067</v>
       </c>
       <c r="C145" t="inlineStr">
         <is>
@@ -2632,7 +2632,7 @@
         </is>
       </c>
       <c r="B147" t="n">
-        <v>419348</v>
+        <v>420301</v>
       </c>
       <c r="C147" t="inlineStr">
         <is>
@@ -2647,7 +2647,7 @@
         </is>
       </c>
       <c r="B148" t="n">
-        <v>40433</v>
+        <v>40464</v>
       </c>
       <c r="C148" t="inlineStr">
         <is>
@@ -2662,7 +2662,7 @@
         </is>
       </c>
       <c r="B149" t="n">
-        <v>691920</v>
+        <v>693169</v>
       </c>
       <c r="C149" t="inlineStr">
         <is>
@@ -2677,7 +2677,7 @@
         </is>
       </c>
       <c r="B150" t="n">
-        <v>5873</v>
+        <v>6373</v>
       </c>
       <c r="C150" t="inlineStr">
         <is>
@@ -2707,7 +2707,7 @@
         </is>
       </c>
       <c r="B152" t="n">
-        <v>61218</v>
+        <v>61235</v>
       </c>
       <c r="C152" t="inlineStr">
         <is>
@@ -2722,7 +2722,7 @@
         </is>
       </c>
       <c r="B153" t="n">
-        <v>383098</v>
+        <v>383228</v>
       </c>
       <c r="C153" t="inlineStr">
         <is>
@@ -2737,7 +2737,7 @@
         </is>
       </c>
       <c r="B154" t="n">
-        <v>241672</v>
+        <v>241883</v>
       </c>
       <c r="C154" t="inlineStr">
         <is>
@@ -2782,7 +2782,7 @@
         </is>
       </c>
       <c r="B157" t="n">
-        <v>1584064</v>
+        <v>1584961</v>
       </c>
       <c r="C157" t="inlineStr">
         <is>
@@ -2797,7 +2797,7 @@
         </is>
       </c>
       <c r="B158" t="n">
-        <v>10583</v>
+        <v>10602</v>
       </c>
       <c r="C158" t="inlineStr">
         <is>
@@ -2812,7 +2812,7 @@
         </is>
       </c>
       <c r="B159" t="n">
-        <v>3524077</v>
+        <v>3540430</v>
       </c>
       <c r="C159" t="inlineStr">
         <is>
@@ -2827,7 +2827,7 @@
         </is>
       </c>
       <c r="B160" t="n">
-        <v>111753</v>
+        <v>113676</v>
       </c>
       <c r="C160" t="inlineStr">
         <is>
@@ -2857,7 +2857,7 @@
         </is>
       </c>
       <c r="B162" t="n">
-        <v>10489</v>
+        <v>10543</v>
       </c>
       <c r="C162" t="inlineStr">
         <is>
@@ -2887,7 +2887,7 @@
         </is>
       </c>
       <c r="B164" t="n">
-        <v>659974</v>
+        <v>663952</v>
       </c>
       <c r="C164" t="inlineStr">
         <is>
@@ -2902,7 +2902,7 @@
         </is>
       </c>
       <c r="B165" t="n">
-        <v>22898</v>
+        <v>22977</v>
       </c>
       <c r="C165" t="inlineStr">
         <is>
@@ -2917,7 +2917,7 @@
         </is>
       </c>
       <c r="B166" t="n">
-        <v>1137</v>
+        <v>1145</v>
       </c>
       <c r="C166" t="inlineStr">
         <is>
@@ -2962,7 +2962,7 @@
         </is>
       </c>
       <c r="B169" t="n">
-        <v>68984</v>
+        <v>71025</v>
       </c>
       <c r="C169" t="inlineStr">
         <is>
@@ -2977,7 +2977,7 @@
         </is>
       </c>
       <c r="B170" t="n">
-        <v>2444</v>
+        <v>2524</v>
       </c>
       <c r="C170" t="inlineStr">
         <is>
@@ -3007,7 +3007,7 @@
         </is>
       </c>
       <c r="B172" t="n">
-        <v>11313</v>
+        <v>11471</v>
       </c>
       <c r="C172" t="inlineStr">
         <is>
@@ -3022,7 +3022,7 @@
         </is>
       </c>
       <c r="B173" t="n">
-        <v>311743</v>
+        <v>312747</v>
       </c>
       <c r="C173" t="inlineStr">
         <is>
@@ -3037,7 +3037,7 @@
         </is>
       </c>
       <c r="B174" t="n">
-        <v>4875388</v>
+        <v>4900121</v>
       </c>
       <c r="C174" t="inlineStr">
         <is>
@@ -3052,7 +3052,7 @@
         </is>
       </c>
       <c r="B175" t="n">
-        <v>32421641</v>
+        <v>32472201</v>
       </c>
       <c r="C175" t="inlineStr">
         <is>
@@ -3067,7 +3067,7 @@
         </is>
       </c>
       <c r="B176" t="n">
-        <v>41905</v>
+        <v>41973</v>
       </c>
       <c r="C176" t="inlineStr">
         <is>
@@ -3082,7 +3082,7 @@
         </is>
       </c>
       <c r="B177" t="n">
-        <v>2137959</v>
+        <v>2140838</v>
       </c>
       <c r="C177" t="inlineStr">
         <is>
@@ -3097,7 +3097,7 @@
         </is>
       </c>
       <c r="B178" t="n">
-        <v>523795</v>
+        <v>525567</v>
       </c>
       <c r="C178" t="inlineStr">
         <is>
@@ -3112,7 +3112,7 @@
         </is>
       </c>
       <c r="B179" t="n">
-        <v>4435831</v>
+        <v>4437505</v>
       </c>
       <c r="C179" t="inlineStr">
         <is>
@@ -3127,7 +3127,7 @@
         </is>
       </c>
       <c r="B180" t="n">
-        <v>202492</v>
+        <v>204120</v>
       </c>
       <c r="C180" t="inlineStr">
         <is>
@@ -3142,7 +3142,7 @@
         </is>
       </c>
       <c r="B181" t="n">
-        <v>91643</v>
+        <v>92006</v>
       </c>
       <c r="C181" t="inlineStr">
         <is>
@@ -3172,7 +3172,7 @@
         </is>
       </c>
       <c r="B183" t="n">
-        <v>200067</v>
+        <v>200931</v>
       </c>
       <c r="C183" t="inlineStr">
         <is>
@@ -3187,7 +3187,7 @@
         </is>
       </c>
       <c r="B184" t="n">
-        <v>2962</v>
+        <v>2985</v>
       </c>
       <c r="C184" t="inlineStr">
         <is>
@@ -3202,7 +3202,7 @@
         </is>
       </c>
       <c r="B185" t="n">
-        <v>297638</v>
+        <v>298203</v>
       </c>
       <c r="C185" t="inlineStr">
         <is>
@@ -3217,7 +3217,7 @@
         </is>
       </c>
       <c r="B186" t="n">
-        <v>6341</v>
+        <v>6363</v>
       </c>
       <c r="C186" t="inlineStr">
         <is>
@@ -3232,7 +3232,7 @@
         </is>
       </c>
       <c r="B187" t="n">
-        <v>91693</v>
+        <v>91722</v>
       </c>
       <c r="C187" t="inlineStr">
         <is>
@@ -3247,7 +3247,7 @@
         </is>
       </c>
       <c r="B188" t="n">
-        <v>38281</v>
+        <v>38293</v>
       </c>
       <c r="C188" t="inlineStr">
         <is>

</xml_diff>